<commit_message>
db connection and scenarios added
</commit_message>
<xml_diff>
--- a/src/main/resources/master_xml.xlsx
+++ b/src/main/resources/master_xml.xlsx
@@ -12,18 +12,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
   <si>
     <t>num</t>
   </si>
   <si>
+    <t>gid</t>
+  </si>
+  <si>
+    <t>lang</t>
+  </si>
+  <si>
     <t>title</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t/>
+    <t>3095466740</t>
+  </si>
+  <si>
+    <t>EN</t>
   </si>
   <si>
     <t>The Battlefield the Girl Saw</t>
@@ -32,70 +41,106 @@
     <t>2</t>
   </si>
   <si>
+    <t>1019682570</t>
+  </si>
+  <si>
     <t>The Trail of Tears</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
+    <t>2879327918</t>
+  </si>
+  <si>
     <t>Quality and Quantity</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
+    <t>1042118304</t>
+  </si>
+  <si>
     <t>Encounter</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
+    <t>1323093475</t>
+  </si>
+  <si>
     <t>Foes and Friends</t>
   </si>
   <si>
     <t>6</t>
   </si>
   <si>
+    <t>3023688674</t>
+  </si>
+  <si>
     <t>The Black Operator</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
+    <t>2322922310</t>
+  </si>
+  <si>
     <t>Fulfilled Ambition</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
+    <t>1400916808</t>
+  </si>
+  <si>
     <t>The Silver-winged Visitor</t>
   </si>
   <si>
     <t>9</t>
   </si>
   <si>
+    <t>2204235069</t>
+  </si>
+  <si>
     <t>The Game's Winner</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
+    <t>2038411104</t>
+  </si>
+  <si>
     <t>Red and Black</t>
   </si>
   <si>
     <t>11</t>
   </si>
   <si>
+    <t>250690944</t>
+  </si>
+  <si>
     <t>Family</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
+    <t>1897449103</t>
+  </si>
+  <si>
     <t>Blue and Red</t>
   </si>
   <si>
     <t>13</t>
+  </si>
+  <si>
+    <t>1997989660</t>
   </si>
   <si>
     <t>And Then</t>
@@ -143,7 +188,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -156,109 +201,193 @@
       <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
+      <c r="C1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>19</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>16</v>
+        <v>24</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>31</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>22</v>
+        <v>33</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>24</v>
+        <v>36</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>37</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>26</v>
+        <v>39</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>40</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>28</v>
+        <v>42</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>